<commit_message>
checked thrown alerts by hand, starting on new tool
</commit_message>
<xml_diff>
--- a/bugs_table.xlsx
+++ b/bugs_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxbe\Desktop\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6CA44-DE50-488A-BC4B-F61503EBC69A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EC9A45-2D93-4050-A38B-1F2D96927399}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88C54D22-CC6D-44EB-88DB-9A6383E82FD2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$K$380</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$K$383</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$O:$O</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1765" uniqueCount="279">
   <si>
     <t>File</t>
   </si>
@@ -1222,15 +1222,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEEF99E-85B6-452B-AB09-1A7819E6A45F}">
-  <dimension ref="A1:Q380"/>
+  <dimension ref="A1:Q383"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="S385" sqref="S378:U385"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C230" sqref="C230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" style="1" customWidth="1"/>
@@ -3567,45 +3567,42 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B107" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C107">
-        <v>192</v>
+        <v>423</v>
       </c>
       <c r="D107" t="s">
-        <v>221</v>
-      </c>
-      <c r="E107" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="H107" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B108" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C108">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="D108" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="H108" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
@@ -3613,19 +3610,22 @@
         <v>238</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C109">
-        <v>439</v>
+        <v>192</v>
       </c>
       <c r="D109" t="s">
+        <v>221</v>
+      </c>
+      <c r="E109" t="s">
         <v>222</v>
       </c>
       <c r="H109" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
@@ -3636,7 +3636,7 @@
         <v>66</v>
       </c>
       <c r="C110">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="D110" t="s">
         <v>222</v>
@@ -3656,16 +3656,16 @@
         <v>66</v>
       </c>
       <c r="C111">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D111" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="H111" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
@@ -3676,16 +3676,16 @@
         <v>66</v>
       </c>
       <c r="C112">
-        <v>462</v>
+        <v>442</v>
       </c>
       <c r="D112" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="H112" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
@@ -3696,16 +3696,16 @@
         <v>66</v>
       </c>
       <c r="C113">
-        <v>492</v>
+        <v>446</v>
       </c>
       <c r="D113" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="H113" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
@@ -3713,21 +3713,15 @@
         <v>238</v>
       </c>
       <c r="B114" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C114">
-        <v>889</v>
+        <v>462</v>
       </c>
       <c r="D114" t="s">
-        <v>216</v>
-      </c>
-      <c r="E114" t="s">
         <v>215</v>
       </c>
       <c r="H114" t="s">
-        <v>10</v>
-      </c>
-      <c r="I114" t="s">
         <v>4</v>
       </c>
       <c r="K114" s="1" t="s">
@@ -3739,25 +3733,19 @@
         <v>238</v>
       </c>
       <c r="B115" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C115">
-        <v>931</v>
+        <v>492</v>
       </c>
       <c r="D115" t="s">
-        <v>216</v>
-      </c>
-      <c r="E115" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="H115" t="s">
-        <v>10</v>
-      </c>
-      <c r="I115" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
@@ -3768,7 +3756,7 @@
         <v>68</v>
       </c>
       <c r="C116">
-        <v>970</v>
+        <v>889</v>
       </c>
       <c r="D116" t="s">
         <v>216</v>
@@ -3794,7 +3782,7 @@
         <v>68</v>
       </c>
       <c r="C117">
-        <v>971</v>
+        <v>931</v>
       </c>
       <c r="D117" t="s">
         <v>216</v>
@@ -3820,16 +3808,13 @@
         <v>68</v>
       </c>
       <c r="C118">
-        <v>978</v>
+        <v>970</v>
       </c>
       <c r="D118" t="s">
         <v>216</v>
       </c>
       <c r="E118" t="s">
-        <v>226</v>
-      </c>
-      <c r="F118" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H118" t="s">
         <v>10</v>
@@ -3843,36 +3828,57 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B119" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C119">
-        <v>2774</v>
+        <v>971</v>
+      </c>
+      <c r="D119" t="s">
+        <v>216</v>
+      </c>
+      <c r="E119" t="s">
+        <v>215</v>
       </c>
       <c r="H119" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="I119" t="s">
+        <v>4</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B120" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C120">
-        <v>2782</v>
+        <v>978</v>
+      </c>
+      <c r="D120" t="s">
+        <v>216</v>
+      </c>
+      <c r="E120" t="s">
+        <v>226</v>
+      </c>
+      <c r="F120" t="s">
+        <v>224</v>
       </c>
       <c r="H120" t="s">
-        <v>18</v>
+        <v>10</v>
+      </c>
+      <c r="I120" t="s">
+        <v>4</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.3">
@@ -3883,7 +3889,7 @@
         <v>69</v>
       </c>
       <c r="C121">
-        <v>2796</v>
+        <v>2774</v>
       </c>
       <c r="H121" t="s">
         <v>18</v>
@@ -3900,7 +3906,7 @@
         <v>69</v>
       </c>
       <c r="C122">
-        <v>2814</v>
+        <v>2782</v>
       </c>
       <c r="H122" t="s">
         <v>18</v>
@@ -3917,7 +3923,7 @@
         <v>69</v>
       </c>
       <c r="C123">
-        <v>2821</v>
+        <v>2796</v>
       </c>
       <c r="H123" t="s">
         <v>18</v>
@@ -3934,7 +3940,7 @@
         <v>69</v>
       </c>
       <c r="C124">
-        <v>2822</v>
+        <v>2814</v>
       </c>
       <c r="H124" t="s">
         <v>18</v>
@@ -3945,36 +3951,36 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B125" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C125">
-        <v>878</v>
+        <v>2821</v>
       </c>
       <c r="H125" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B126" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C126">
-        <v>914</v>
+        <v>2822</v>
       </c>
       <c r="H126" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
@@ -3985,7 +3991,7 @@
         <v>71</v>
       </c>
       <c r="C127">
-        <v>1062</v>
+        <v>878</v>
       </c>
       <c r="H127" t="s">
         <v>10</v>
@@ -4002,7 +4008,7 @@
         <v>71</v>
       </c>
       <c r="C128">
-        <v>1073</v>
+        <v>914</v>
       </c>
       <c r="H128" t="s">
         <v>10</v>
@@ -4016,16 +4022,16 @@
         <v>240</v>
       </c>
       <c r="B129" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C129">
-        <v>3758</v>
+        <v>1062</v>
       </c>
       <c r="H129" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.3">
@@ -4033,50 +4039,50 @@
         <v>240</v>
       </c>
       <c r="B130" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C130">
-        <v>3920</v>
+        <v>1073</v>
       </c>
       <c r="H130" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B131" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C131">
-        <v>370</v>
+        <v>3758</v>
       </c>
       <c r="H131" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B132" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C132">
-        <v>372</v>
+        <v>3920</v>
       </c>
       <c r="H132" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.3">
@@ -4084,10 +4090,10 @@
         <v>241</v>
       </c>
       <c r="B133" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C133">
-        <v>417</v>
+        <v>370</v>
       </c>
       <c r="H133" t="s">
         <v>64</v>
@@ -4101,10 +4107,10 @@
         <v>241</v>
       </c>
       <c r="B134" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C134">
-        <v>426</v>
+        <v>372</v>
       </c>
       <c r="H134" t="s">
         <v>64</v>
@@ -4121,7 +4127,7 @@
         <v>76</v>
       </c>
       <c r="C135">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="H135" t="s">
         <v>64</v>
@@ -4138,7 +4144,7 @@
         <v>76</v>
       </c>
       <c r="C136">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="H136" t="s">
         <v>64</v>
@@ -4152,10 +4158,10 @@
         <v>241</v>
       </c>
       <c r="B137" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C137">
-        <v>506</v>
+        <v>428</v>
       </c>
       <c r="H137" t="s">
         <v>64</v>
@@ -4169,10 +4175,10 @@
         <v>241</v>
       </c>
       <c r="B138" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C138">
-        <v>518</v>
+        <v>430</v>
       </c>
       <c r="H138" t="s">
         <v>64</v>
@@ -4189,7 +4195,7 @@
         <v>77</v>
       </c>
       <c r="C139">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="H139" t="s">
         <v>64</v>
@@ -4206,7 +4212,7 @@
         <v>77</v>
       </c>
       <c r="C140">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="H140" t="s">
         <v>64</v>
@@ -4220,16 +4226,16 @@
         <v>241</v>
       </c>
       <c r="B141" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C141">
-        <v>672</v>
+        <v>520</v>
       </c>
       <c r="H141" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.3">
@@ -4237,50 +4243,50 @@
         <v>241</v>
       </c>
       <c r="B142" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C142">
-        <v>673</v>
+        <v>522</v>
       </c>
       <c r="H142" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B143" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C143">
-        <v>1136</v>
+        <v>672</v>
       </c>
       <c r="H143" t="s">
-        <v>85</v>
-      </c>
-      <c r="I143" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B144" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C144">
-        <v>1160</v>
+        <v>673</v>
+      </c>
+      <c r="H144" t="s">
+        <v>34</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.3">
@@ -4288,13 +4294,19 @@
         <v>242</v>
       </c>
       <c r="B145" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C145">
-        <v>1160</v>
+        <v>1136</v>
+      </c>
+      <c r="H145" t="s">
+        <v>85</v>
+      </c>
+      <c r="I145" t="s">
+        <v>4</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
@@ -4305,7 +4317,7 @@
         <v>84</v>
       </c>
       <c r="C146">
-        <v>1293</v>
+        <v>1160</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>82</v>
@@ -4319,16 +4331,10 @@
         <v>84</v>
       </c>
       <c r="C147">
-        <v>1300</v>
-      </c>
-      <c r="H147" t="s">
-        <v>85</v>
-      </c>
-      <c r="I147" t="s">
-        <v>4</v>
+        <v>1160</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
@@ -4339,16 +4345,10 @@
         <v>84</v>
       </c>
       <c r="C148">
-        <v>1302</v>
-      </c>
-      <c r="H148" t="s">
-        <v>85</v>
-      </c>
-      <c r="I148" t="s">
-        <v>4</v>
+        <v>1293</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
@@ -4359,7 +4359,7 @@
         <v>84</v>
       </c>
       <c r="C149">
-        <v>1307</v>
+        <v>1300</v>
       </c>
       <c r="H149" t="s">
         <v>85</v>
@@ -4379,7 +4379,7 @@
         <v>84</v>
       </c>
       <c r="C150">
-        <v>1309</v>
+        <v>1302</v>
       </c>
       <c r="H150" t="s">
         <v>85</v>
@@ -4399,10 +4399,16 @@
         <v>84</v>
       </c>
       <c r="C151">
-        <v>1300</v>
+        <v>1307</v>
+      </c>
+      <c r="H151" t="s">
+        <v>85</v>
+      </c>
+      <c r="I151" t="s">
+        <v>4</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
@@ -4413,10 +4419,16 @@
         <v>84</v>
       </c>
       <c r="C152">
-        <v>1302</v>
+        <v>1309</v>
+      </c>
+      <c r="H152" t="s">
+        <v>85</v>
+      </c>
+      <c r="I152" t="s">
+        <v>4</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
@@ -4427,7 +4439,7 @@
         <v>84</v>
       </c>
       <c r="C153">
-        <v>1307</v>
+        <v>1300</v>
       </c>
       <c r="K153" s="1" t="s">
         <v>82</v>
@@ -4441,7 +4453,7 @@
         <v>84</v>
       </c>
       <c r="C154">
-        <v>1309</v>
+        <v>1302</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>82</v>
@@ -4455,10 +4467,10 @@
         <v>84</v>
       </c>
       <c r="C155">
-        <v>1321</v>
+        <v>1307</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.3">
@@ -4469,10 +4481,10 @@
         <v>84</v>
       </c>
       <c r="C156">
-        <v>1323</v>
+        <v>1309</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
@@ -4483,7 +4495,7 @@
         <v>84</v>
       </c>
       <c r="C157">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="K157" s="1" t="s">
         <v>83</v>
@@ -4497,7 +4509,7 @@
         <v>84</v>
       </c>
       <c r="C158">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="K158" s="1" t="s">
         <v>83</v>
@@ -4511,16 +4523,10 @@
         <v>84</v>
       </c>
       <c r="C159">
-        <v>1321</v>
-      </c>
-      <c r="H159" t="s">
-        <v>85</v>
-      </c>
-      <c r="I159" t="s">
-        <v>4</v>
+        <v>1327</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
@@ -4531,16 +4537,10 @@
         <v>84</v>
       </c>
       <c r="C160">
-        <v>1323</v>
-      </c>
-      <c r="H160" t="s">
-        <v>85</v>
-      </c>
-      <c r="I160" t="s">
-        <v>4</v>
+        <v>1329</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.3">
@@ -4551,7 +4551,7 @@
         <v>84</v>
       </c>
       <c r="C161">
-        <v>1327</v>
+        <v>1321</v>
       </c>
       <c r="H161" t="s">
         <v>85</v>
@@ -4571,7 +4571,7 @@
         <v>84</v>
       </c>
       <c r="C162">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="H162" t="s">
         <v>85</v>
@@ -4588,19 +4588,19 @@
         <v>242</v>
       </c>
       <c r="B163" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C163">
-        <v>1636</v>
+        <v>1327</v>
       </c>
       <c r="H163" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="I163" t="s">
         <v>4</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.3">
@@ -4608,19 +4608,19 @@
         <v>242</v>
       </c>
       <c r="B164" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C164">
-        <v>1649</v>
+        <v>1329</v>
       </c>
       <c r="H164" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="I164" t="s">
         <v>4</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
@@ -4631,7 +4631,7 @@
         <v>87</v>
       </c>
       <c r="C165">
-        <v>1650</v>
+        <v>1636</v>
       </c>
       <c r="H165" t="s">
         <v>10</v>
@@ -4645,36 +4645,42 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B166" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C166">
-        <v>185</v>
+        <v>1649</v>
       </c>
       <c r="H166" t="s">
         <v>10</v>
       </c>
+      <c r="I166" t="s">
+        <v>4</v>
+      </c>
       <c r="K166" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B167" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C167">
-        <v>244</v>
+        <v>1650</v>
       </c>
       <c r="H167" t="s">
         <v>10</v>
       </c>
+      <c r="I167" t="s">
+        <v>4</v>
+      </c>
       <c r="K167" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.3">
@@ -4685,7 +4691,7 @@
         <v>88</v>
       </c>
       <c r="C168">
-        <v>248</v>
+        <v>185</v>
       </c>
       <c r="H168" t="s">
         <v>10</v>
@@ -4696,36 +4702,36 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>243</v>
+      </c>
+      <c r="B169" t="s">
+        <v>88</v>
+      </c>
+      <c r="C169">
         <v>244</v>
       </c>
-      <c r="B169" t="s">
-        <v>91</v>
-      </c>
-      <c r="C169">
-        <v>388</v>
-      </c>
       <c r="H169" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="K169" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B170" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C170">
-        <v>390</v>
+        <v>248</v>
       </c>
       <c r="H170" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="K170" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.3">
@@ -4736,10 +4742,10 @@
         <v>91</v>
       </c>
       <c r="C171">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="H171" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K171" s="1" t="s">
         <v>93</v>
@@ -4753,10 +4759,10 @@
         <v>91</v>
       </c>
       <c r="C172">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="H172" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K172" s="1" t="s">
         <v>93</v>
@@ -4764,36 +4770,36 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B173" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C173">
-        <v>453</v>
+        <v>394</v>
       </c>
       <c r="H173" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="K173" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B174" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C174">
-        <v>494</v>
+        <v>399</v>
       </c>
       <c r="H174" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.3">
@@ -4804,7 +4810,7 @@
         <v>96</v>
       </c>
       <c r="C175">
-        <v>501</v>
+        <v>453</v>
       </c>
       <c r="H175" t="s">
         <v>64</v>
@@ -4821,7 +4827,7 @@
         <v>96</v>
       </c>
       <c r="C176">
-        <v>547</v>
+        <v>494</v>
       </c>
       <c r="H176" t="s">
         <v>64</v>
@@ -4838,7 +4844,7 @@
         <v>96</v>
       </c>
       <c r="C177">
-        <v>562</v>
+        <v>501</v>
       </c>
       <c r="H177" t="s">
         <v>64</v>
@@ -4855,7 +4861,7 @@
         <v>96</v>
       </c>
       <c r="C178">
-        <v>611</v>
+        <v>547</v>
       </c>
       <c r="H178" t="s">
         <v>64</v>
@@ -4866,42 +4872,36 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B179" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C179">
-        <v>1332</v>
+        <v>562</v>
       </c>
       <c r="H179" t="s">
-        <v>10</v>
-      </c>
-      <c r="I179" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K179" s="1" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B180" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C180">
-        <v>2204</v>
+        <v>611</v>
       </c>
       <c r="H180" t="s">
-        <v>10</v>
-      </c>
-      <c r="I180" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="K180" s="1" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.3">
@@ -4909,10 +4909,10 @@
         <v>246</v>
       </c>
       <c r="B181" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C181">
-        <v>2327</v>
+        <v>1332</v>
       </c>
       <c r="H181" t="s">
         <v>10</v>
@@ -4932,7 +4932,7 @@
         <v>99</v>
       </c>
       <c r="C182">
-        <v>2467</v>
+        <v>2204</v>
       </c>
       <c r="H182" t="s">
         <v>10</v>
@@ -4952,7 +4952,7 @@
         <v>99</v>
       </c>
       <c r="C183">
-        <v>2468</v>
+        <v>2327</v>
       </c>
       <c r="H183" t="s">
         <v>10</v>
@@ -4972,7 +4972,7 @@
         <v>99</v>
       </c>
       <c r="C184">
-        <v>2471</v>
+        <v>2467</v>
       </c>
       <c r="H184" t="s">
         <v>10</v>
@@ -4992,7 +4992,7 @@
         <v>99</v>
       </c>
       <c r="C185">
-        <v>2479</v>
+        <v>2468</v>
       </c>
       <c r="H185" t="s">
         <v>10</v>
@@ -5012,7 +5012,7 @@
         <v>99</v>
       </c>
       <c r="C186">
-        <v>2483</v>
+        <v>2471</v>
       </c>
       <c r="H186" t="s">
         <v>10</v>
@@ -5032,7 +5032,7 @@
         <v>99</v>
       </c>
       <c r="C187">
-        <v>2509</v>
+        <v>2479</v>
       </c>
       <c r="H187" t="s">
         <v>10</v>
@@ -5052,7 +5052,7 @@
         <v>99</v>
       </c>
       <c r="C188">
-        <v>2553</v>
+        <v>2483</v>
       </c>
       <c r="H188" t="s">
         <v>10</v>
@@ -5072,7 +5072,7 @@
         <v>99</v>
       </c>
       <c r="C189">
-        <v>2577</v>
+        <v>2509</v>
       </c>
       <c r="H189" t="s">
         <v>10</v>
@@ -5092,7 +5092,7 @@
         <v>99</v>
       </c>
       <c r="C190">
-        <v>2593</v>
+        <v>2553</v>
       </c>
       <c r="H190" t="s">
         <v>10</v>
@@ -5106,36 +5106,42 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B191" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C191">
-        <v>606</v>
+        <v>2577</v>
       </c>
       <c r="H191" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="I191" t="s">
+        <v>100</v>
       </c>
       <c r="K191" s="1" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B192" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C192">
-        <v>638</v>
+        <v>2593</v>
       </c>
       <c r="H192" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="I192" t="s">
+        <v>100</v>
       </c>
       <c r="K192" s="1" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.3">
@@ -5146,7 +5152,7 @@
         <v>101</v>
       </c>
       <c r="C193">
-        <v>646</v>
+        <v>606</v>
       </c>
       <c r="H193" t="s">
         <v>12</v>
@@ -5157,36 +5163,36 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B194" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C194">
-        <v>197</v>
+        <v>638</v>
       </c>
       <c r="H194" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K194" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B195" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C195">
-        <v>198</v>
+        <v>646</v>
       </c>
       <c r="H195" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K195" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.3">
@@ -5197,7 +5203,7 @@
         <v>103</v>
       </c>
       <c r="C196">
-        <v>225</v>
+        <v>197</v>
       </c>
       <c r="H196" t="s">
         <v>34</v>
@@ -5214,7 +5220,7 @@
         <v>103</v>
       </c>
       <c r="C197">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="H197" t="s">
         <v>34</v>
@@ -5231,7 +5237,7 @@
         <v>103</v>
       </c>
       <c r="C198">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="H198" t="s">
         <v>34</v>
@@ -5248,7 +5254,7 @@
         <v>103</v>
       </c>
       <c r="C199">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H199" t="s">
         <v>34</v>
@@ -5265,7 +5271,7 @@
         <v>103</v>
       </c>
       <c r="C200">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="H200" t="s">
         <v>34</v>
@@ -5276,98 +5282,104 @@
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B201" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C201">
-        <v>700</v>
+        <v>248</v>
       </c>
       <c r="H201" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K201" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B202" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C202">
-        <v>702</v>
+        <v>253</v>
       </c>
       <c r="H202" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K202" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B203" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C203">
-        <v>5869</v>
+        <v>700</v>
       </c>
       <c r="H203" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="K203" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B204" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C204">
-        <v>5872</v>
+        <v>702</v>
       </c>
       <c r="H204" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="K204" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B205" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C205">
-        <v>251</v>
+        <v>5869</v>
+      </c>
+      <c r="H205" t="s">
+        <v>108</v>
       </c>
       <c r="K205" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B206" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C206">
-        <v>262</v>
+        <v>5872</v>
+      </c>
+      <c r="H206" t="s">
+        <v>108</v>
       </c>
       <c r="K206" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.3">
@@ -5375,104 +5387,95 @@
         <v>251</v>
       </c>
       <c r="B207" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C207">
-        <v>910</v>
-      </c>
-      <c r="H207" t="s">
-        <v>113</v>
+        <v>251</v>
       </c>
       <c r="K207" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B208" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C208">
-        <v>2258</v>
-      </c>
-      <c r="H208" t="s">
-        <v>22</v>
+        <v>262</v>
       </c>
       <c r="K208" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B209" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C209">
-        <v>297</v>
+        <v>910</v>
       </c>
       <c r="H209" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="K209" s="1" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B210" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C210">
-        <v>571</v>
+        <v>2258</v>
       </c>
       <c r="H210" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K210" s="1" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B211" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C211">
-        <v>4024</v>
+        <v>297</v>
       </c>
       <c r="H211" t="s">
-        <v>119</v>
-      </c>
-      <c r="I211" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="K211" s="1" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B212" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C212">
-        <v>4509</v>
+        <v>571</v>
       </c>
       <c r="H212" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="K212" s="1" t="s">
-        <v>122</v>
+        <v>19</v>
       </c>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.3">
@@ -5480,50 +5483,53 @@
         <v>254</v>
       </c>
       <c r="B213" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C213">
-        <v>4529</v>
+        <v>4024</v>
       </c>
       <c r="H213" t="s">
-        <v>4</v>
+        <v>119</v>
+      </c>
+      <c r="I213" t="s">
+        <v>45</v>
       </c>
       <c r="K213" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B214" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C214">
-        <v>500</v>
+        <v>4509</v>
       </c>
       <c r="H214" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="K214" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B215" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C215">
-        <v>503</v>
+        <v>4529</v>
       </c>
       <c r="H215" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="K215" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.3">
@@ -5534,7 +5540,7 @@
         <v>123</v>
       </c>
       <c r="C216">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="H216" t="s">
         <v>124</v>
@@ -5551,7 +5557,7 @@
         <v>123</v>
       </c>
       <c r="C217">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="H217" t="s">
         <v>124</v>
@@ -5568,7 +5574,7 @@
         <v>123</v>
       </c>
       <c r="C218">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="H218" t="s">
         <v>124</v>
@@ -5585,7 +5591,7 @@
         <v>123</v>
       </c>
       <c r="C219">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="H219" t="s">
         <v>124</v>
@@ -5602,7 +5608,7 @@
         <v>123</v>
       </c>
       <c r="C220">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="H220" t="s">
         <v>124</v>
@@ -5619,7 +5625,7 @@
         <v>123</v>
       </c>
       <c r="C221">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="H221" t="s">
         <v>124</v>
@@ -5636,7 +5642,7 @@
         <v>123</v>
       </c>
       <c r="C222">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="H222" t="s">
         <v>124</v>
@@ -5653,7 +5659,7 @@
         <v>123</v>
       </c>
       <c r="C223">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="H223" t="s">
         <v>124</v>
@@ -5670,7 +5676,7 @@
         <v>123</v>
       </c>
       <c r="C224">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="H224" t="s">
         <v>124</v>
@@ -5687,7 +5693,7 @@
         <v>123</v>
       </c>
       <c r="C225">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="H225" t="s">
         <v>124</v>
@@ -5701,10 +5707,10 @@
         <v>255</v>
       </c>
       <c r="B226" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C226">
-        <v>581</v>
+        <v>530</v>
       </c>
       <c r="H226" t="s">
         <v>124</v>
@@ -5718,70 +5724,67 @@
         <v>255</v>
       </c>
       <c r="B227" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C227">
-        <v>942</v>
+        <v>533</v>
       </c>
       <c r="H227" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="K227" s="1" t="s">
-        <v>39</v>
+        <v>125</v>
       </c>
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B228" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C228">
-        <v>642</v>
+        <v>581</v>
       </c>
       <c r="H228" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K228" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B229" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C229">
-        <v>650</v>
+        <v>583</v>
       </c>
       <c r="H229" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K229" s="1" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B230" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C230">
-        <v>758</v>
+        <v>942</v>
       </c>
       <c r="H230" t="s">
-        <v>124</v>
-      </c>
-      <c r="I230" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="K230" s="1" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.3">
@@ -5789,19 +5792,16 @@
         <v>256</v>
       </c>
       <c r="B231" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C231">
-        <v>760</v>
+        <v>642</v>
       </c>
       <c r="H231" t="s">
-        <v>124</v>
-      </c>
-      <c r="I231" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="K231" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.3">
@@ -5809,19 +5809,16 @@
         <v>256</v>
       </c>
       <c r="B232" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C232">
-        <v>761</v>
+        <v>650</v>
       </c>
       <c r="H232" t="s">
-        <v>124</v>
-      </c>
-      <c r="I232" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="K232" s="1" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.3">
@@ -5829,16 +5826,19 @@
         <v>256</v>
       </c>
       <c r="B233" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C233">
-        <v>1145</v>
+        <v>758</v>
       </c>
       <c r="H233" t="s">
-        <v>64</v>
+        <v>124</v>
+      </c>
+      <c r="I233" t="s">
+        <v>4</v>
       </c>
       <c r="K233" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.3">
@@ -5846,87 +5846,84 @@
         <v>256</v>
       </c>
       <c r="B234" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C234">
-        <v>1290</v>
+        <v>760</v>
       </c>
       <c r="H234" t="s">
-        <v>64</v>
+        <v>124</v>
+      </c>
+      <c r="I234" t="s">
+        <v>4</v>
       </c>
       <c r="K234" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B235" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C235">
-        <v>2740</v>
+        <v>761</v>
       </c>
       <c r="H235" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="I235" t="s">
         <v>4</v>
       </c>
       <c r="K235" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B236" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C236">
-        <v>2743</v>
+        <v>1145</v>
       </c>
       <c r="H236" t="s">
-        <v>92</v>
-      </c>
-      <c r="I236" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K236" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B237" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C237">
-        <v>2746</v>
+        <v>1290</v>
       </c>
       <c r="H237" t="s">
-        <v>92</v>
-      </c>
-      <c r="I237" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K237" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B238" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C238">
-        <v>930</v>
+        <v>2740</v>
       </c>
       <c r="H238" t="s">
         <v>92</v>
@@ -5935,18 +5932,18 @@
         <v>4</v>
       </c>
       <c r="K238" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B239" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C239">
-        <v>938</v>
+        <v>2743</v>
       </c>
       <c r="H239" t="s">
         <v>92</v>
@@ -5955,58 +5952,67 @@
         <v>4</v>
       </c>
       <c r="K239" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B240" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C240">
-        <v>935</v>
+        <v>2746</v>
       </c>
       <c r="H240" t="s">
-        <v>12</v>
+        <v>92</v>
+      </c>
+      <c r="I240" t="s">
+        <v>4</v>
       </c>
       <c r="K240" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B241" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C241">
-        <v>1071</v>
+        <v>930</v>
       </c>
       <c r="H241" t="s">
-        <v>12</v>
+        <v>92</v>
+      </c>
+      <c r="I241" t="s">
+        <v>4</v>
       </c>
       <c r="K241" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B242" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C242">
-        <v>1078</v>
+        <v>938</v>
       </c>
       <c r="H242" t="s">
-        <v>12</v>
+        <v>92</v>
+      </c>
+      <c r="I242" t="s">
+        <v>4</v>
       </c>
       <c r="K242" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.3">
@@ -6014,10 +6020,10 @@
         <v>259</v>
       </c>
       <c r="B243" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C243">
-        <v>1079</v>
+        <v>935</v>
       </c>
       <c r="H243" t="s">
         <v>12</v>
@@ -6034,7 +6040,7 @@
         <v>141</v>
       </c>
       <c r="C244">
-        <v>1089</v>
+        <v>1071</v>
       </c>
       <c r="H244" t="s">
         <v>12</v>
@@ -6051,7 +6057,7 @@
         <v>141</v>
       </c>
       <c r="C245">
-        <v>1201</v>
+        <v>1078</v>
       </c>
       <c r="H245" t="s">
         <v>12</v>
@@ -6065,10 +6071,10 @@
         <v>259</v>
       </c>
       <c r="B246" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C246">
-        <v>2665</v>
+        <v>1079</v>
       </c>
       <c r="H246" t="s">
         <v>12</v>
@@ -6082,10 +6088,10 @@
         <v>259</v>
       </c>
       <c r="B247" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C247">
-        <v>2666</v>
+        <v>1089</v>
       </c>
       <c r="H247" t="s">
         <v>12</v>
@@ -6096,53 +6102,53 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B248" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C248">
-        <v>4536</v>
+        <v>1201</v>
       </c>
       <c r="H248" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K248" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B249" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C249">
-        <v>4567</v>
+        <v>2665</v>
       </c>
       <c r="H249" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K249" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B250" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C250">
-        <v>4591</v>
+        <v>2666</v>
       </c>
       <c r="H250" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="K250" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.3">
@@ -6150,10 +6156,10 @@
         <v>260</v>
       </c>
       <c r="B251" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C251">
-        <v>4651</v>
+        <v>4536</v>
       </c>
       <c r="H251" t="s">
         <v>34</v>
@@ -6167,10 +6173,10 @@
         <v>260</v>
       </c>
       <c r="B252" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C252">
-        <v>4652</v>
+        <v>4567</v>
       </c>
       <c r="H252" t="s">
         <v>34</v>
@@ -6184,10 +6190,10 @@
         <v>260</v>
       </c>
       <c r="B253" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C253">
-        <v>5389</v>
+        <v>4591</v>
       </c>
       <c r="H253" t="s">
         <v>34</v>
@@ -6198,50 +6204,50 @@
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B254" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C254">
-        <v>462</v>
+        <v>4651</v>
       </c>
       <c r="H254" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K254" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B255" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C255">
-        <v>470</v>
+        <v>4652</v>
       </c>
       <c r="H255" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="K255" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B256" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C256">
-        <v>1629</v>
+        <v>5389</v>
       </c>
       <c r="H256" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="K256" s="1" t="s">
         <v>144</v>
@@ -6252,85 +6258,67 @@
         <v>261</v>
       </c>
       <c r="B257" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C257">
-        <v>1677</v>
+        <v>462</v>
       </c>
       <c r="H257" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="K257" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B258" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C258">
-        <v>2705</v>
+        <v>470</v>
       </c>
       <c r="H258" t="s">
-        <v>124</v>
-      </c>
-      <c r="I258" t="s">
-        <v>124</v>
-      </c>
-      <c r="J258" t="s">
-        <v>157</v>
+        <v>12</v>
       </c>
       <c r="K258" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B259" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C259">
-        <v>2791</v>
+        <v>1629</v>
       </c>
       <c r="H259" t="s">
-        <v>124</v>
-      </c>
-      <c r="I259" t="s">
-        <v>124</v>
-      </c>
-      <c r="J259" t="s">
-        <v>157</v>
+        <v>64</v>
       </c>
       <c r="K259" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B260" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C260">
-        <v>2792</v>
+        <v>1677</v>
       </c>
       <c r="H260" t="s">
-        <v>124</v>
-      </c>
-      <c r="I260" t="s">
-        <v>124</v>
-      </c>
-      <c r="J260" t="s">
-        <v>157</v>
+        <v>64</v>
       </c>
       <c r="K260" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.3">
@@ -6341,7 +6329,7 @@
         <v>152</v>
       </c>
       <c r="C261">
-        <v>2795</v>
+        <v>2705</v>
       </c>
       <c r="H261" t="s">
         <v>124</v>
@@ -6361,10 +6349,10 @@
         <v>262</v>
       </c>
       <c r="B262" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C262">
-        <v>2879</v>
+        <v>2791</v>
       </c>
       <c r="H262" t="s">
         <v>124</v>
@@ -6384,10 +6372,10 @@
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C263">
-        <v>2882</v>
+        <v>2792</v>
       </c>
       <c r="H263" t="s">
         <v>124</v>
@@ -6407,13 +6395,13 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C264">
-        <v>3169</v>
+        <v>2795</v>
       </c>
       <c r="H264" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="I264" t="s">
         <v>124</v>
@@ -6430,13 +6418,13 @@
         <v>262</v>
       </c>
       <c r="B265" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C265">
-        <v>3170</v>
+        <v>2879</v>
       </c>
       <c r="H265" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="I265" t="s">
         <v>124</v>
@@ -6453,13 +6441,13 @@
         <v>262</v>
       </c>
       <c r="B266" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C266">
-        <v>3175</v>
+        <v>2882</v>
       </c>
       <c r="H266" t="s">
-        <v>34</v>
+        <v>124</v>
       </c>
       <c r="I266" t="s">
         <v>124</v>
@@ -6479,7 +6467,7 @@
         <v>155</v>
       </c>
       <c r="C267">
-        <v>3176</v>
+        <v>3169</v>
       </c>
       <c r="H267" t="s">
         <v>34</v>
@@ -6496,121 +6484,139 @@
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B268" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C268">
-        <v>908</v>
+        <v>3170</v>
       </c>
       <c r="H268" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="I268" t="s">
+        <v>124</v>
+      </c>
+      <c r="J268" t="s">
+        <v>157</v>
       </c>
       <c r="K268" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B269" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C269">
-        <v>971</v>
+        <v>3175</v>
       </c>
       <c r="H269" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="I269" t="s">
+        <v>124</v>
+      </c>
+      <c r="J269" t="s">
+        <v>157</v>
       </c>
       <c r="K269" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B270" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C270">
-        <v>3116</v>
+        <v>3176</v>
       </c>
       <c r="H270" t="s">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="I270" t="s">
+        <v>124</v>
+      </c>
+      <c r="J270" t="s">
+        <v>157</v>
       </c>
       <c r="K270" s="1" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B271" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C271">
-        <v>3117</v>
+        <v>908</v>
       </c>
       <c r="H271" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K271" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B272" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C272">
-        <v>880</v>
+        <v>971</v>
       </c>
       <c r="H272" t="s">
-        <v>163</v>
+        <v>12</v>
       </c>
       <c r="K272" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B273" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C273">
-        <v>897</v>
+        <v>3116</v>
       </c>
       <c r="H273" t="s">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="K273" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B274" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C274">
-        <v>906</v>
+        <v>3117</v>
       </c>
       <c r="H274" t="s">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="K274" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.3">
@@ -6621,7 +6627,7 @@
         <v>162</v>
       </c>
       <c r="C275">
-        <v>913</v>
+        <v>880</v>
       </c>
       <c r="H275" t="s">
         <v>163</v>
@@ -6638,7 +6644,7 @@
         <v>162</v>
       </c>
       <c r="C276">
-        <v>1005</v>
+        <v>897</v>
       </c>
       <c r="H276" t="s">
         <v>163</v>
@@ -6652,76 +6658,67 @@
         <v>265</v>
       </c>
       <c r="B277" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C277">
-        <v>1628</v>
+        <v>906</v>
       </c>
       <c r="H277" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K277" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B278" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C278">
-        <v>1440</v>
+        <v>913</v>
       </c>
       <c r="H278" t="s">
-        <v>168</v>
-      </c>
-      <c r="I278" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K278" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B279" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C279">
-        <v>5774</v>
+        <v>1005</v>
       </c>
       <c r="H279" t="s">
-        <v>168</v>
-      </c>
-      <c r="I279" t="s">
-        <v>22</v>
+        <v>163</v>
       </c>
       <c r="K279" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B280" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C280">
-        <v>5778</v>
+        <v>1628</v>
       </c>
       <c r="H280" t="s">
-        <v>168</v>
-      </c>
-      <c r="I280" t="s">
         <v>22</v>
       </c>
       <c r="K280" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.3">
@@ -6729,10 +6726,10 @@
         <v>266</v>
       </c>
       <c r="B281" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C281">
-        <v>5880</v>
+        <v>1440</v>
       </c>
       <c r="H281" t="s">
         <v>168</v>
@@ -6746,53 +6743,62 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B282" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C282">
-        <v>2765</v>
+        <v>5774</v>
       </c>
       <c r="H282" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="I282" t="s">
+        <v>22</v>
       </c>
       <c r="K282" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B283" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C283">
-        <v>2781</v>
+        <v>5778</v>
       </c>
       <c r="H283" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="I283" t="s">
+        <v>22</v>
       </c>
       <c r="K283" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B284" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C284">
-        <v>2786</v>
+        <v>5880</v>
       </c>
       <c r="H284" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="I284" t="s">
+        <v>22</v>
       </c>
       <c r="K284" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.3">
@@ -6803,7 +6809,7 @@
         <v>171</v>
       </c>
       <c r="C285">
-        <v>2787</v>
+        <v>2765</v>
       </c>
       <c r="H285" t="s">
         <v>173</v>
@@ -6820,7 +6826,7 @@
         <v>171</v>
       </c>
       <c r="C286">
-        <v>2790</v>
+        <v>2781</v>
       </c>
       <c r="H286" t="s">
         <v>173</v>
@@ -6837,7 +6843,7 @@
         <v>171</v>
       </c>
       <c r="C287">
-        <v>2792</v>
+        <v>2786</v>
       </c>
       <c r="H287" t="s">
         <v>173</v>
@@ -6848,71 +6854,53 @@
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B288" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C288">
-        <v>371</v>
+        <v>2787</v>
       </c>
       <c r="H288" t="s">
-        <v>176</v>
-      </c>
-      <c r="I288" t="s">
-        <v>177</v>
-      </c>
-      <c r="J288" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K288" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B289" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C289">
-        <v>385</v>
+        <v>2790</v>
       </c>
       <c r="H289" t="s">
-        <v>176</v>
-      </c>
-      <c r="I289" t="s">
-        <v>177</v>
-      </c>
-      <c r="J289" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K289" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B290" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C290">
-        <v>419</v>
+        <v>2792</v>
       </c>
       <c r="H290" t="s">
-        <v>176</v>
-      </c>
-      <c r="I290" t="s">
-        <v>177</v>
-      </c>
-      <c r="J290" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K290" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
@@ -6923,7 +6911,7 @@
         <v>174</v>
       </c>
       <c r="C291">
-        <v>426</v>
+        <v>371</v>
       </c>
       <c r="H291" t="s">
         <v>176</v>
@@ -6940,53 +6928,71 @@
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B292" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C292">
-        <v>2107</v>
+        <v>385</v>
       </c>
       <c r="H292" t="s">
-        <v>64</v>
+        <v>176</v>
+      </c>
+      <c r="I292" t="s">
+        <v>177</v>
+      </c>
+      <c r="J292" t="s">
+        <v>178</v>
       </c>
       <c r="K292" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B293" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C293">
-        <v>2126</v>
+        <v>419</v>
       </c>
       <c r="H293" t="s">
-        <v>64</v>
+        <v>176</v>
+      </c>
+      <c r="I293" t="s">
+        <v>177</v>
+      </c>
+      <c r="J293" t="s">
+        <v>178</v>
       </c>
       <c r="K293" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B294" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C294">
-        <v>8210</v>
+        <v>426</v>
       </c>
       <c r="H294" t="s">
-        <v>64</v>
+        <v>176</v>
+      </c>
+      <c r="I294" t="s">
+        <v>177</v>
+      </c>
+      <c r="J294" t="s">
+        <v>178</v>
       </c>
       <c r="K294" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.3">
@@ -6994,16 +7000,16 @@
         <v>269</v>
       </c>
       <c r="B295" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C295">
-        <v>8430</v>
+        <v>2107</v>
       </c>
       <c r="H295" t="s">
         <v>64</v>
       </c>
       <c r="K295" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.3">
@@ -7011,16 +7017,16 @@
         <v>269</v>
       </c>
       <c r="B296" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C296">
-        <v>8455</v>
+        <v>2126</v>
       </c>
       <c r="H296" t="s">
         <v>64</v>
       </c>
       <c r="K296" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
@@ -7028,10 +7034,10 @@
         <v>269</v>
       </c>
       <c r="B297" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C297">
-        <v>8522</v>
+        <v>8210</v>
       </c>
       <c r="H297" t="s">
         <v>64</v>
@@ -7045,16 +7051,16 @@
         <v>269</v>
       </c>
       <c r="B298" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C298">
-        <v>8631</v>
+        <v>8430</v>
       </c>
       <c r="H298" t="s">
         <v>64</v>
       </c>
       <c r="K298" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
@@ -7062,16 +7068,16 @@
         <v>269</v>
       </c>
       <c r="B299" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C299">
-        <v>8684</v>
+        <v>8455</v>
       </c>
       <c r="H299" t="s">
         <v>64</v>
       </c>
       <c r="K299" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
@@ -7082,7 +7088,7 @@
         <v>185</v>
       </c>
       <c r="C300">
-        <v>8684</v>
+        <v>8522</v>
       </c>
       <c r="H300" t="s">
         <v>64</v>
@@ -7091,38 +7097,38 @@
         <v>181</v>
       </c>
     </row>
-    <row r="301" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>269</v>
       </c>
-      <c r="B301" s="2" t="s">
-        <v>186</v>
+      <c r="B301" t="s">
+        <v>185</v>
       </c>
       <c r="C301">
-        <v>10389</v>
+        <v>8631</v>
       </c>
       <c r="H301" t="s">
         <v>64</v>
       </c>
       <c r="K301" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="302" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>269</v>
       </c>
-      <c r="B302" s="2" t="s">
-        <v>186</v>
+      <c r="B302" t="s">
+        <v>185</v>
       </c>
       <c r="C302">
-        <v>10399</v>
+        <v>8684</v>
       </c>
       <c r="H302" t="s">
         <v>64</v>
       </c>
       <c r="K302" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.3">
@@ -7130,27 +7136,27 @@
         <v>269</v>
       </c>
       <c r="B303" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C303">
-        <v>10499</v>
+        <v>8684</v>
       </c>
       <c r="H303" t="s">
         <v>64</v>
       </c>
       <c r="K303" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>269</v>
       </c>
-      <c r="B304" t="s">
-        <v>188</v>
+      <c r="B304" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="C304">
-        <v>10500</v>
+        <v>10389</v>
       </c>
       <c r="H304" t="s">
         <v>64</v>
@@ -7159,15 +7165,15 @@
         <v>187</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>269</v>
       </c>
-      <c r="B305" t="s">
-        <v>188</v>
+      <c r="B305" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="C305">
-        <v>10596</v>
+        <v>10399</v>
       </c>
       <c r="H305" t="s">
         <v>64</v>
@@ -7184,7 +7190,7 @@
         <v>188</v>
       </c>
       <c r="C306">
-        <v>10597</v>
+        <v>10499</v>
       </c>
       <c r="H306" t="s">
         <v>64</v>
@@ -7198,16 +7204,16 @@
         <v>269</v>
       </c>
       <c r="B307" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C307">
-        <v>2107</v>
+        <v>10500</v>
       </c>
       <c r="H307" t="s">
         <v>64</v>
       </c>
       <c r="K307" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.3">
@@ -7215,16 +7221,16 @@
         <v>269</v>
       </c>
       <c r="B308" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C308">
-        <v>2126</v>
+        <v>10596</v>
       </c>
       <c r="H308" t="s">
         <v>64</v>
       </c>
       <c r="K308" s="1" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.3">
@@ -7232,16 +7238,16 @@
         <v>269</v>
       </c>
       <c r="B309" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C309">
-        <v>8210</v>
+        <v>10597</v>
       </c>
       <c r="H309" t="s">
         <v>64</v>
       </c>
       <c r="K309" s="1" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.3">
@@ -7249,16 +7255,16 @@
         <v>269</v>
       </c>
       <c r="B310" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C310">
-        <v>8430</v>
+        <v>2107</v>
       </c>
       <c r="H310" t="s">
         <v>64</v>
       </c>
       <c r="K310" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.3">
@@ -7266,16 +7272,16 @@
         <v>269</v>
       </c>
       <c r="B311" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C311">
-        <v>8455</v>
+        <v>2126</v>
       </c>
       <c r="H311" t="s">
         <v>64</v>
       </c>
       <c r="K311" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.3">
@@ -7283,10 +7289,10 @@
         <v>269</v>
       </c>
       <c r="B312" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C312">
-        <v>8522</v>
+        <v>8210</v>
       </c>
       <c r="H312" t="s">
         <v>64</v>
@@ -7300,16 +7306,16 @@
         <v>269</v>
       </c>
       <c r="B313" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C313">
-        <v>8631</v>
+        <v>8430</v>
       </c>
       <c r="H313" t="s">
         <v>64</v>
       </c>
       <c r="K313" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.3">
@@ -7317,16 +7323,16 @@
         <v>269</v>
       </c>
       <c r="B314" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C314">
-        <v>8684</v>
+        <v>8455</v>
       </c>
       <c r="H314" t="s">
         <v>64</v>
       </c>
       <c r="K314" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.3">
@@ -7337,7 +7343,7 @@
         <v>185</v>
       </c>
       <c r="C315">
-        <v>8700</v>
+        <v>8522</v>
       </c>
       <c r="H315" t="s">
         <v>64</v>
@@ -7351,16 +7357,16 @@
         <v>269</v>
       </c>
       <c r="B316" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C316">
-        <v>10389</v>
+        <v>8631</v>
       </c>
       <c r="H316" t="s">
         <v>64</v>
       </c>
       <c r="K316" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
@@ -7368,16 +7374,16 @@
         <v>269</v>
       </c>
       <c r="B317" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C317">
-        <v>10399</v>
+        <v>8684</v>
       </c>
       <c r="H317" t="s">
         <v>64</v>
       </c>
       <c r="K317" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.3">
@@ -7385,16 +7391,16 @@
         <v>269</v>
       </c>
       <c r="B318" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C318">
-        <v>10499</v>
+        <v>8700</v>
       </c>
       <c r="H318" t="s">
         <v>64</v>
       </c>
       <c r="K318" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.3">
@@ -7405,7 +7411,7 @@
         <v>188</v>
       </c>
       <c r="C319">
-        <v>10500</v>
+        <v>10389</v>
       </c>
       <c r="H319" t="s">
         <v>64</v>
@@ -7422,7 +7428,7 @@
         <v>188</v>
       </c>
       <c r="C320">
-        <v>10596</v>
+        <v>10399</v>
       </c>
       <c r="H320" t="s">
         <v>64</v>
@@ -7439,7 +7445,7 @@
         <v>188</v>
       </c>
       <c r="C321">
-        <v>10597</v>
+        <v>10499</v>
       </c>
       <c r="H321" t="s">
         <v>64</v>
@@ -7450,70 +7456,70 @@
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B322" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C322">
-        <v>943</v>
+        <v>10500</v>
       </c>
       <c r="H322" t="s">
         <v>64</v>
       </c>
       <c r="K322" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
     </row>
     <row r="323" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B323" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C323">
-        <v>275</v>
+        <v>10596</v>
       </c>
       <c r="H323" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K323" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B324" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C324">
-        <v>692</v>
+        <v>10597</v>
       </c>
       <c r="H324" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K324" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="325" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B325" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C325">
-        <v>715</v>
+        <v>943</v>
       </c>
       <c r="H325" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="K325" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="326" spans="1:11" x14ac:dyDescent="0.3">
@@ -7521,10 +7527,10 @@
         <v>271</v>
       </c>
       <c r="B326" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C326">
-        <v>735</v>
+        <v>275</v>
       </c>
       <c r="H326" t="s">
         <v>4</v>
@@ -7538,10 +7544,10 @@
         <v>271</v>
       </c>
       <c r="B327" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C327">
-        <v>1328</v>
+        <v>692</v>
       </c>
       <c r="H327" t="s">
         <v>4</v>
@@ -7555,10 +7561,10 @@
         <v>271</v>
       </c>
       <c r="B328" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C328">
-        <v>1356</v>
+        <v>715</v>
       </c>
       <c r="H328" t="s">
         <v>4</v>
@@ -7572,10 +7578,10 @@
         <v>271</v>
       </c>
       <c r="B329" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C329">
-        <v>1401</v>
+        <v>735</v>
       </c>
       <c r="H329" t="s">
         <v>4</v>
@@ -7592,7 +7598,7 @@
         <v>193</v>
       </c>
       <c r="C330">
-        <v>1482</v>
+        <v>1328</v>
       </c>
       <c r="H330" t="s">
         <v>4</v>
@@ -7609,7 +7615,7 @@
         <v>193</v>
       </c>
       <c r="C331">
-        <v>1485</v>
+        <v>1356</v>
       </c>
       <c r="H331" t="s">
         <v>4</v>
@@ -7626,7 +7632,7 @@
         <v>193</v>
       </c>
       <c r="C332">
-        <v>1497</v>
+        <v>1401</v>
       </c>
       <c r="H332" t="s">
         <v>4</v>
@@ -7643,7 +7649,7 @@
         <v>193</v>
       </c>
       <c r="C333">
-        <v>1582</v>
+        <v>1482</v>
       </c>
       <c r="H333" t="s">
         <v>4</v>
@@ -7657,10 +7663,10 @@
         <v>271</v>
       </c>
       <c r="B334" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C334">
-        <v>1620</v>
+        <v>1485</v>
       </c>
       <c r="H334" t="s">
         <v>4</v>
@@ -7674,10 +7680,10 @@
         <v>271</v>
       </c>
       <c r="B335" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C335">
-        <v>1682</v>
+        <v>1497</v>
       </c>
       <c r="H335" t="s">
         <v>4</v>
@@ -7691,10 +7697,10 @@
         <v>271</v>
       </c>
       <c r="B336" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C336">
-        <v>1694</v>
+        <v>1582</v>
       </c>
       <c r="H336" t="s">
         <v>4</v>
@@ -7708,10 +7714,10 @@
         <v>271</v>
       </c>
       <c r="B337" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C337">
-        <v>1793</v>
+        <v>1620</v>
       </c>
       <c r="H337" t="s">
         <v>4</v>
@@ -7725,10 +7731,10 @@
         <v>271</v>
       </c>
       <c r="B338" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C338">
-        <v>1801</v>
+        <v>1682</v>
       </c>
       <c r="H338" t="s">
         <v>4</v>
@@ -7739,184 +7745,175 @@
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B339" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C339">
-        <v>2045</v>
+        <v>1694</v>
       </c>
       <c r="H339" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K339" s="1" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B340" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C340">
-        <v>2070</v>
+        <v>1793</v>
       </c>
       <c r="H340" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K340" s="1" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B341" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C341">
-        <v>2071</v>
+        <v>1801</v>
       </c>
       <c r="H341" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K341" s="1" t="s">
-        <v>43</v>
+        <v>190</v>
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B342" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C342">
-        <v>1506</v>
+        <v>2045</v>
       </c>
       <c r="H342" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K342" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B343" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C343">
-        <v>1515</v>
+        <v>2070</v>
       </c>
       <c r="H343" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K343" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B344" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C344">
-        <v>195</v>
+        <v>2071</v>
       </c>
       <c r="H344" t="s">
         <v>10</v>
       </c>
-      <c r="I344" t="s">
-        <v>4</v>
-      </c>
       <c r="K344" s="1" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B345" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C345">
-        <v>411</v>
+        <v>1506</v>
       </c>
       <c r="H345" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K345" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B346" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C346">
-        <v>797</v>
+        <v>1515</v>
       </c>
       <c r="H346" t="s">
-        <v>204</v>
-      </c>
-      <c r="I346" t="s">
-        <v>205</v>
+        <v>12</v>
       </c>
       <c r="K346" s="1" t="s">
-        <v>203</v>
+        <v>48</v>
       </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B347" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C347">
-        <v>805</v>
+        <v>195</v>
       </c>
       <c r="H347" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
       <c r="I347" t="s">
-        <v>205</v>
+        <v>4</v>
       </c>
       <c r="K347" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B348" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C348">
-        <v>809</v>
+        <v>411</v>
       </c>
       <c r="H348" t="s">
-        <v>204</v>
-      </c>
-      <c r="I348" t="s">
-        <v>205</v>
+        <v>10</v>
       </c>
       <c r="K348" s="1" t="s">
-        <v>203</v>
+        <v>9</v>
       </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.3">
@@ -7927,7 +7924,7 @@
         <v>202</v>
       </c>
       <c r="C349">
-        <v>811</v>
+        <v>797</v>
       </c>
       <c r="H349" t="s">
         <v>204</v>
@@ -7941,53 +7938,62 @@
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B350" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C350">
-        <v>161</v>
+        <v>805</v>
       </c>
       <c r="H350" t="s">
-        <v>56</v>
+        <v>204</v>
+      </c>
+      <c r="I350" t="s">
+        <v>205</v>
       </c>
       <c r="K350" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B351" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C351">
-        <v>171</v>
+        <v>809</v>
       </c>
       <c r="H351" t="s">
-        <v>56</v>
+        <v>204</v>
+      </c>
+      <c r="I351" t="s">
+        <v>205</v>
       </c>
       <c r="K351" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B352" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C352">
-        <v>181</v>
+        <v>811</v>
       </c>
       <c r="H352" t="s">
-        <v>56</v>
+        <v>204</v>
+      </c>
+      <c r="I352" t="s">
+        <v>205</v>
       </c>
       <c r="K352" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.3">
@@ -7998,7 +8004,7 @@
         <v>207</v>
       </c>
       <c r="C353">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="H353" t="s">
         <v>56</v>
@@ -8015,7 +8021,7 @@
         <v>207</v>
       </c>
       <c r="C354">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="H354" t="s">
         <v>56</v>
@@ -8032,7 +8038,7 @@
         <v>207</v>
       </c>
       <c r="C355">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="H355" t="s">
         <v>56</v>
@@ -8049,7 +8055,7 @@
         <v>207</v>
       </c>
       <c r="C356">
-        <v>248</v>
+        <v>184</v>
       </c>
       <c r="H356" t="s">
         <v>56</v>
@@ -8066,7 +8072,7 @@
         <v>207</v>
       </c>
       <c r="C357">
-        <v>261</v>
+        <v>202</v>
       </c>
       <c r="H357" t="s">
         <v>56</v>
@@ -8080,10 +8086,10 @@
         <v>277</v>
       </c>
       <c r="B358" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C358">
-        <v>433</v>
+        <v>205</v>
       </c>
       <c r="H358" t="s">
         <v>56</v>
@@ -8094,53 +8100,53 @@
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B359" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C359">
-        <v>673</v>
+        <v>248</v>
       </c>
       <c r="H359" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="K359" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B360" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C360">
-        <v>673</v>
+        <v>261</v>
       </c>
       <c r="H360" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="K360" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B361" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C361">
-        <v>686</v>
+        <v>433</v>
       </c>
       <c r="H361" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="K361" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.3">
@@ -8151,13 +8157,13 @@
         <v>209</v>
       </c>
       <c r="C362">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="H362" t="s">
         <v>85</v>
       </c>
       <c r="K362" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.3">
@@ -8168,13 +8174,13 @@
         <v>209</v>
       </c>
       <c r="C363">
-        <v>693</v>
+        <v>673</v>
       </c>
       <c r="H363" t="s">
         <v>85</v>
       </c>
       <c r="K363" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.3">
@@ -8185,13 +8191,13 @@
         <v>209</v>
       </c>
       <c r="C364">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="H364" t="s">
         <v>85</v>
       </c>
       <c r="K364" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.3">
@@ -8202,13 +8208,13 @@
         <v>209</v>
       </c>
       <c r="C365">
-        <v>697</v>
+        <v>687</v>
       </c>
       <c r="H365" t="s">
         <v>85</v>
       </c>
       <c r="K365" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.3">
@@ -8219,13 +8225,13 @@
         <v>209</v>
       </c>
       <c r="C366">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="H366" t="s">
         <v>85</v>
       </c>
       <c r="K366" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.3">
@@ -8236,13 +8242,13 @@
         <v>209</v>
       </c>
       <c r="C367">
-        <v>710</v>
+        <v>694</v>
       </c>
       <c r="H367" t="s">
         <v>85</v>
       </c>
       <c r="K367" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.3">
@@ -8253,13 +8259,13 @@
         <v>209</v>
       </c>
       <c r="C368">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="H368" t="s">
         <v>85</v>
       </c>
       <c r="K368" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.3">
@@ -8270,13 +8276,13 @@
         <v>209</v>
       </c>
       <c r="C369">
-        <v>717</v>
+        <v>697</v>
       </c>
       <c r="H369" t="s">
         <v>85</v>
       </c>
       <c r="K369" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.3">
@@ -8287,13 +8293,13 @@
         <v>209</v>
       </c>
       <c r="C370">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="H370" t="s">
         <v>85</v>
       </c>
       <c r="K370" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.3">
@@ -8304,13 +8310,13 @@
         <v>209</v>
       </c>
       <c r="C371">
-        <v>734</v>
+        <v>711</v>
       </c>
       <c r="H371" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="K371" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.3">
@@ -8321,7 +8327,7 @@
         <v>209</v>
       </c>
       <c r="C372">
-        <v>739</v>
+        <v>717</v>
       </c>
       <c r="H372" t="s">
         <v>85</v>
@@ -8338,7 +8344,7 @@
         <v>209</v>
       </c>
       <c r="C373">
-        <v>739</v>
+        <v>718</v>
       </c>
       <c r="H373" t="s">
         <v>85</v>
@@ -8352,16 +8358,16 @@
         <v>278</v>
       </c>
       <c r="B374" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C374">
-        <v>841</v>
+        <v>734</v>
       </c>
       <c r="H374" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="K374" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.3">
@@ -8369,16 +8375,16 @@
         <v>278</v>
       </c>
       <c r="B375" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C375">
-        <v>850</v>
+        <v>739</v>
       </c>
       <c r="H375" t="s">
         <v>85</v>
       </c>
       <c r="K375" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.3">
@@ -8386,10 +8392,10 @@
         <v>278</v>
       </c>
       <c r="B376" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C376">
-        <v>852</v>
+        <v>739</v>
       </c>
       <c r="H376" t="s">
         <v>85</v>
@@ -8403,16 +8409,16 @@
         <v>278</v>
       </c>
       <c r="B377" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C377">
-        <v>855</v>
+        <v>841</v>
       </c>
       <c r="H377" t="s">
         <v>85</v>
       </c>
       <c r="K377" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.3">
@@ -8420,16 +8426,16 @@
         <v>278</v>
       </c>
       <c r="B378" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C378">
-        <v>868</v>
+        <v>850</v>
       </c>
       <c r="H378" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="K378" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.3">
@@ -8437,16 +8443,16 @@
         <v>278</v>
       </c>
       <c r="B379" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C379">
-        <v>872</v>
+        <v>852</v>
       </c>
       <c r="H379" t="s">
         <v>85</v>
       </c>
       <c r="K379" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.3">
@@ -8457,12 +8463,63 @@
         <v>209</v>
       </c>
       <c r="C380">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="H380" t="s">
         <v>85</v>
       </c>
       <c r="K380" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>278</v>
+      </c>
+      <c r="B381" t="s">
+        <v>209</v>
+      </c>
+      <c r="C381">
+        <v>868</v>
+      </c>
+      <c r="H381" t="s">
+        <v>64</v>
+      </c>
+      <c r="K381" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>278</v>
+      </c>
+      <c r="B382" t="s">
+        <v>209</v>
+      </c>
+      <c r="C382">
+        <v>872</v>
+      </c>
+      <c r="H382" t="s">
+        <v>85</v>
+      </c>
+      <c r="K382" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>278</v>
+      </c>
+      <c r="B383" t="s">
+        <v>209</v>
+      </c>
+      <c r="C383">
+        <v>872</v>
+      </c>
+      <c r="H383" t="s">
+        <v>85</v>
+      </c>
+      <c r="K383" s="1" t="s">
         <v>211</v>
       </c>
     </row>

</xml_diff>

<commit_message>
finished numbering bug progression in truth table
</commit_message>
<xml_diff>
--- a/bugs_table.xlsx
+++ b/bugs_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maxbe\Desktop\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1AF5BA-36C5-48A9-ABAB-C5E3DC81A24C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7305B9-6DE3-46E5-B514-B8085A32B00C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88C54D22-CC6D-44EB-88DB-9A6383E82FD2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$K$388</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$K$373</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$O:$O</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1792" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="280">
   <si>
     <t>File</t>
   </si>
@@ -1225,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEEF99E-85B6-452B-AB09-1A7819E6A45F}">
-  <dimension ref="A1:Q388"/>
+  <dimension ref="A1:Q373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScale="91" workbookViewId="0">
-      <selection activeCell="L276" sqref="L276"/>
+    <sheetView tabSelected="1" topLeftCell="A346" zoomScale="91" workbookViewId="0">
+      <selection activeCell="L374" sqref="L374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7492,13 +7492,16 @@
         <v>158</v>
       </c>
       <c r="C276">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="H276" t="s">
         <v>12</v>
       </c>
       <c r="K276" s="1" t="s">
         <v>159</v>
+      </c>
+      <c r="L276">
+        <v>1</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.3">
@@ -7517,6 +7520,9 @@
       <c r="K277" s="1" t="s">
         <v>159</v>
       </c>
+      <c r="L277">
+        <v>2</v>
+      </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
@@ -7534,6 +7540,9 @@
       <c r="K278" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="L278">
+        <v>2</v>
+      </c>
     </row>
     <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
@@ -7551,6 +7560,9 @@
       <c r="K279" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="L279">
+        <v>1</v>
+      </c>
     </row>
     <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
@@ -7568,6 +7580,9 @@
       <c r="K280" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="L280">
+        <v>1</v>
+      </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
@@ -7585,6 +7600,9 @@
       <c r="K281" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="L281">
+        <v>2</v>
+      </c>
     </row>
     <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
@@ -7602,6 +7620,9 @@
       <c r="K282" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="L282">
+        <v>3</v>
+      </c>
     </row>
     <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
@@ -7619,6 +7640,9 @@
       <c r="K283" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="L283">
+        <v>4</v>
+      </c>
     </row>
     <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
@@ -7636,6 +7660,9 @@
       <c r="K284" s="1" t="s">
         <v>164</v>
       </c>
+      <c r="L284">
+        <v>5</v>
+      </c>
     </row>
     <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
@@ -7653,6 +7680,9 @@
       <c r="K285" s="1" t="s">
         <v>166</v>
       </c>
+      <c r="L285">
+        <v>4</v>
+      </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
@@ -7673,6 +7703,9 @@
       <c r="K286" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="L286">
+        <v>5</v>
+      </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
@@ -7693,6 +7726,9 @@
       <c r="K287" s="1" t="s">
         <v>169</v>
       </c>
+      <c r="L287">
+        <v>1</v>
+      </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
@@ -7713,8 +7749,11 @@
       <c r="K288" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L288">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>266</v>
       </c>
@@ -7733,8 +7772,11 @@
       <c r="K289" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L289">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>267</v>
       </c>
@@ -7750,8 +7792,11 @@
       <c r="K290" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>267</v>
       </c>
@@ -7767,8 +7812,11 @@
       <c r="K291" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>267</v>
       </c>
@@ -7784,8 +7832,11 @@
       <c r="K292" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L292">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>267</v>
       </c>
@@ -7801,8 +7852,11 @@
       <c r="K293" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L293">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>267</v>
       </c>
@@ -7818,8 +7872,11 @@
       <c r="K294" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L294">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>267</v>
       </c>
@@ -7835,8 +7892,11 @@
       <c r="K295" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L295">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>268</v>
       </c>
@@ -7858,8 +7918,11 @@
       <c r="K296" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>268</v>
       </c>
@@ -7881,8 +7944,11 @@
       <c r="K297" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>268</v>
       </c>
@@ -7904,8 +7970,11 @@
       <c r="K298" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L298">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>268</v>
       </c>
@@ -7927,8 +7996,11 @@
       <c r="K299" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L299">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>269</v>
       </c>
@@ -7944,8 +8016,11 @@
       <c r="K300" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>269</v>
       </c>
@@ -7961,8 +8036,11 @@
       <c r="K301" s="1" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L301">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>269</v>
       </c>
@@ -7978,8 +8056,11 @@
       <c r="K302" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L302">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>269</v>
       </c>
@@ -7995,8 +8076,11 @@
       <c r="K303" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>269</v>
       </c>
@@ -8012,8 +8096,11 @@
       <c r="K304" s="1" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L304">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>269</v>
       </c>
@@ -8029,8 +8116,11 @@
       <c r="K305" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>269</v>
       </c>
@@ -8046,8 +8136,11 @@
       <c r="K306" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L306">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>269</v>
       </c>
@@ -8063,8 +8156,11 @@
       <c r="K307" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L307">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>269</v>
       </c>
@@ -8080,8 +8176,11 @@
       <c r="K308" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="309" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L308">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="309" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>269</v>
       </c>
@@ -8097,8 +8196,11 @@
       <c r="K309" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="310" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="L309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>269</v>
       </c>
@@ -8114,8 +8216,11 @@
       <c r="K310" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L310">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>269</v>
       </c>
@@ -8131,8 +8236,11 @@
       <c r="K311" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L311">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>269</v>
       </c>
@@ -8148,8 +8256,11 @@
       <c r="K312" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L312">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>269</v>
       </c>
@@ -8165,8 +8276,11 @@
       <c r="K313" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L313">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>269</v>
       </c>
@@ -8182,288 +8296,339 @@
       <c r="K314" s="1" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L314">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B315" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="C315">
-        <v>2107</v>
+        <v>943</v>
       </c>
       <c r="H315" t="s">
         <v>64</v>
       </c>
       <c r="K315" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+      <c r="L315">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B316" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="C316">
-        <v>2126</v>
+        <v>275</v>
       </c>
       <c r="H316" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K316" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B317" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C317">
-        <v>8210</v>
+        <v>692</v>
       </c>
       <c r="H317" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K317" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L317">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B318" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C318">
-        <v>8430</v>
+        <v>715</v>
       </c>
       <c r="H318" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K318" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L318">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B319" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C319">
-        <v>8455</v>
+        <v>735</v>
       </c>
       <c r="H319" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K319" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L319">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B320" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C320">
-        <v>8522</v>
+        <v>1328</v>
       </c>
       <c r="H320" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K320" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L320">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B321" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C321">
-        <v>8631</v>
+        <v>1356</v>
       </c>
       <c r="H321" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K321" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L321">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B322" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C322">
-        <v>8684</v>
+        <v>1401</v>
       </c>
       <c r="H322" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K322" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L322">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B323" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C323">
-        <v>8700</v>
+        <v>1482</v>
       </c>
       <c r="H323" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K323" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L323">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B324" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C324">
-        <v>10389</v>
+        <v>1485</v>
       </c>
       <c r="H324" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K324" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L324">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B325" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C325">
-        <v>10399</v>
+        <v>1497</v>
       </c>
       <c r="H325" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K325" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L325">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B326" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C326">
-        <v>10499</v>
+        <v>1582</v>
       </c>
       <c r="H326" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K326" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L326">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B327" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C327">
-        <v>10500</v>
+        <v>1620</v>
       </c>
       <c r="H327" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K327" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L327">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B328" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C328">
-        <v>10596</v>
+        <v>1682</v>
       </c>
       <c r="H328" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K328" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L328">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B329" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C329">
-        <v>10597</v>
+        <v>1694</v>
       </c>
       <c r="H329" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K329" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L329">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B330" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C330">
-        <v>943</v>
+        <v>1793</v>
       </c>
       <c r="H330" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="K330" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+      <c r="L330">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>271</v>
       </c>
       <c r="B331" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="C331">
-        <v>275</v>
+        <v>1801</v>
       </c>
       <c r="H331" t="s">
         <v>4</v>
@@ -8471,643 +8636,754 @@
       <c r="K331" s="1" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L331">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B332" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C332">
-        <v>692</v>
+        <v>2045</v>
       </c>
       <c r="H332" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K332" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="L332">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B333" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C333">
-        <v>715</v>
+        <v>2070</v>
       </c>
       <c r="H333" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K333" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="L333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B334" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="C334">
-        <v>735</v>
+        <v>2071</v>
       </c>
       <c r="H334" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K334" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="L334">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B335" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C335">
-        <v>1328</v>
+        <v>1506</v>
       </c>
       <c r="H335" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K335" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="L335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B336" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C336">
-        <v>1356</v>
+        <v>1515</v>
       </c>
       <c r="H336" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K336" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="L336">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B337" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C337">
-        <v>1401</v>
+        <v>195</v>
       </c>
       <c r="H337" t="s">
+        <v>10</v>
+      </c>
+      <c r="I337" t="s">
         <v>4</v>
       </c>
       <c r="K337" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+      <c r="L337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="B338" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="C338">
-        <v>1482</v>
+        <v>411</v>
       </c>
       <c r="H338" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K338" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="L338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B339" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C339">
-        <v>1485</v>
+        <v>797</v>
       </c>
       <c r="H339" t="s">
-        <v>4</v>
+        <v>204</v>
+      </c>
+      <c r="I339" t="s">
+        <v>205</v>
       </c>
       <c r="K339" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="L339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B340" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C340">
-        <v>1497</v>
+        <v>805</v>
       </c>
       <c r="H340" t="s">
-        <v>4</v>
+        <v>204</v>
+      </c>
+      <c r="I340" t="s">
+        <v>205</v>
       </c>
       <c r="K340" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="L340">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B341" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C341">
-        <v>1582</v>
+        <v>809</v>
       </c>
       <c r="H341" t="s">
-        <v>4</v>
+        <v>204</v>
+      </c>
+      <c r="I341" t="s">
+        <v>205</v>
       </c>
       <c r="K341" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="L341">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B342" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="C342">
-        <v>1620</v>
+        <v>811</v>
       </c>
       <c r="H342" t="s">
-        <v>4</v>
+        <v>204</v>
+      </c>
+      <c r="I342" t="s">
+        <v>205</v>
       </c>
       <c r="K342" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+      <c r="L342">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B343" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C343">
-        <v>1682</v>
+        <v>161</v>
       </c>
       <c r="H343" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="K343" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B344" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C344">
-        <v>1694</v>
+        <v>171</v>
       </c>
       <c r="H344" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="K344" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L344">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B345" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C345">
-        <v>1793</v>
+        <v>181</v>
       </c>
       <c r="H345" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="K345" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L345">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="346" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="B346" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C346">
-        <v>1801</v>
+        <v>184</v>
       </c>
       <c r="H346" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="K346" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L346">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B347" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C347">
-        <v>2045</v>
+        <v>202</v>
       </c>
       <c r="H347" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K347" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L347">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B348" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C348">
-        <v>2070</v>
+        <v>205</v>
       </c>
       <c r="H348" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K348" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L348">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="349" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="B349" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="C349">
-        <v>2071</v>
+        <v>248</v>
       </c>
       <c r="H349" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="K349" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L349">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="350" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B350" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C350">
-        <v>1506</v>
+        <v>261</v>
       </c>
       <c r="H350" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="K350" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L350">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="351" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="B351" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C351">
-        <v>1515</v>
+        <v>433</v>
       </c>
       <c r="H351" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="K351" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+      <c r="L351">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="352" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="B352" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C352">
-        <v>195</v>
+        <v>673</v>
       </c>
       <c r="H352" t="s">
-        <v>10</v>
-      </c>
-      <c r="I352" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="K352" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="B353" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="C353">
-        <v>411</v>
+        <v>673</v>
       </c>
       <c r="H353" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="K353" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L353">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B354" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C354">
-        <v>797</v>
+        <v>686</v>
       </c>
       <c r="H354" t="s">
-        <v>204</v>
-      </c>
-      <c r="I354" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="K354" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L354">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B355" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C355">
-        <v>805</v>
+        <v>687</v>
       </c>
       <c r="H355" t="s">
-        <v>204</v>
-      </c>
-      <c r="I355" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="K355" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L355">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B356" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C356">
-        <v>809</v>
+        <v>693</v>
       </c>
       <c r="H356" t="s">
-        <v>204</v>
-      </c>
-      <c r="I356" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="K356" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L356">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B357" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C357">
-        <v>811</v>
+        <v>694</v>
       </c>
       <c r="H357" t="s">
-        <v>204</v>
-      </c>
-      <c r="I357" t="s">
-        <v>205</v>
+        <v>85</v>
       </c>
       <c r="K357" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L357">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B358" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C358">
-        <v>161</v>
+        <v>697</v>
       </c>
       <c r="H358" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K358" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L358">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="359" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B359" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C359">
-        <v>171</v>
+        <v>697</v>
       </c>
       <c r="H359" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K359" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L359">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="360" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B360" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C360">
-        <v>181</v>
+        <v>710</v>
       </c>
       <c r="H360" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K360" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L360">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B361" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C361">
-        <v>184</v>
+        <v>711</v>
       </c>
       <c r="H361" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K361" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L361">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="362" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B362" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C362">
-        <v>202</v>
+        <v>717</v>
       </c>
       <c r="H362" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K362" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L362">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="363" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B363" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C363">
-        <v>205</v>
+        <v>718</v>
       </c>
       <c r="H363" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K363" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L363">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="364" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B364" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C364">
-        <v>248</v>
+        <v>734</v>
       </c>
       <c r="H364" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="K364" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+      <c r="L364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B365" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C365">
-        <v>261</v>
+        <v>739</v>
       </c>
       <c r="H365" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K365" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L365">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="366" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B366" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C366">
-        <v>433</v>
+        <v>739</v>
       </c>
       <c r="H366" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="K366" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L366">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="367" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>278</v>
       </c>
       <c r="B367" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C367">
-        <v>673</v>
+        <v>841</v>
       </c>
       <c r="H367" t="s">
         <v>85</v>
       </c>
       <c r="K367" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L367">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="368" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>278</v>
       </c>
       <c r="B368" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C368">
-        <v>673</v>
+        <v>850</v>
       </c>
       <c r="H368" t="s">
         <v>85</v>
@@ -9115,25 +9391,31 @@
       <c r="K368" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L368">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>278</v>
       </c>
       <c r="B369" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C369">
-        <v>686</v>
+        <v>852</v>
       </c>
       <c r="H369" t="s">
         <v>85</v>
       </c>
       <c r="K369" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+      <c r="L369">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>278</v>
       </c>
@@ -9141,16 +9423,19 @@
         <v>209</v>
       </c>
       <c r="C370">
-        <v>687</v>
+        <v>855</v>
       </c>
       <c r="H370" t="s">
         <v>85</v>
       </c>
       <c r="K370" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L370">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>278</v>
       </c>
@@ -9158,16 +9443,19 @@
         <v>209</v>
       </c>
       <c r="C371">
-        <v>693</v>
+        <v>868</v>
       </c>
       <c r="H371" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="K371" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+      <c r="L371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>278</v>
       </c>
@@ -9175,16 +9463,19 @@
         <v>209</v>
       </c>
       <c r="C372">
-        <v>694</v>
+        <v>872</v>
       </c>
       <c r="H372" t="s">
         <v>85</v>
       </c>
       <c r="K372" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+      <c r="L372">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>278</v>
       </c>
@@ -9192,268 +9483,16 @@
         <v>209</v>
       </c>
       <c r="C373">
-        <v>697</v>
+        <v>872</v>
       </c>
       <c r="H373" t="s">
         <v>85</v>
       </c>
       <c r="K373" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A374" t="s">
-        <v>278</v>
-      </c>
-      <c r="B374" t="s">
-        <v>209</v>
-      </c>
-      <c r="C374">
-        <v>697</v>
-      </c>
-      <c r="H374" t="s">
-        <v>85</v>
-      </c>
-      <c r="K374" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A375" t="s">
-        <v>278</v>
-      </c>
-      <c r="B375" t="s">
-        <v>209</v>
-      </c>
-      <c r="C375">
-        <v>710</v>
-      </c>
-      <c r="H375" t="s">
-        <v>85</v>
-      </c>
-      <c r="K375" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A376" t="s">
-        <v>278</v>
-      </c>
-      <c r="B376" t="s">
-        <v>209</v>
-      </c>
-      <c r="C376">
-        <v>711</v>
-      </c>
-      <c r="H376" t="s">
-        <v>85</v>
-      </c>
-      <c r="K376" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A377" t="s">
-        <v>278</v>
-      </c>
-      <c r="B377" t="s">
-        <v>209</v>
-      </c>
-      <c r="C377">
-        <v>717</v>
-      </c>
-      <c r="H377" t="s">
-        <v>85</v>
-      </c>
-      <c r="K377" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A378" t="s">
-        <v>278</v>
-      </c>
-      <c r="B378" t="s">
-        <v>209</v>
-      </c>
-      <c r="C378">
-        <v>718</v>
-      </c>
-      <c r="H378" t="s">
-        <v>85</v>
-      </c>
-      <c r="K378" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A379" t="s">
-        <v>278</v>
-      </c>
-      <c r="B379" t="s">
-        <v>209</v>
-      </c>
-      <c r="C379">
-        <v>734</v>
-      </c>
-      <c r="H379" t="s">
-        <v>64</v>
-      </c>
-      <c r="K379" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A380" t="s">
-        <v>278</v>
-      </c>
-      <c r="B380" t="s">
-        <v>209</v>
-      </c>
-      <c r="C380">
-        <v>739</v>
-      </c>
-      <c r="H380" t="s">
-        <v>85</v>
-      </c>
-      <c r="K380" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A381" t="s">
-        <v>278</v>
-      </c>
-      <c r="B381" t="s">
-        <v>209</v>
-      </c>
-      <c r="C381">
-        <v>739</v>
-      </c>
-      <c r="H381" t="s">
-        <v>85</v>
-      </c>
-      <c r="K381" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A382" t="s">
-        <v>278</v>
-      </c>
-      <c r="B382" t="s">
-        <v>213</v>
-      </c>
-      <c r="C382">
-        <v>841</v>
-      </c>
-      <c r="H382" t="s">
-        <v>85</v>
-      </c>
-      <c r="K382" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A383" t="s">
-        <v>278</v>
-      </c>
-      <c r="B383" t="s">
-        <v>213</v>
-      </c>
-      <c r="C383">
-        <v>850</v>
-      </c>
-      <c r="H383" t="s">
-        <v>85</v>
-      </c>
-      <c r="K383" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A384" t="s">
-        <v>278</v>
-      </c>
-      <c r="B384" t="s">
-        <v>213</v>
-      </c>
-      <c r="C384">
-        <v>852</v>
-      </c>
-      <c r="H384" t="s">
-        <v>85</v>
-      </c>
-      <c r="K384" s="1" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A385" t="s">
-        <v>278</v>
-      </c>
-      <c r="B385" t="s">
-        <v>209</v>
-      </c>
-      <c r="C385">
-        <v>855</v>
-      </c>
-      <c r="H385" t="s">
-        <v>85</v>
-      </c>
-      <c r="K385" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A386" t="s">
-        <v>278</v>
-      </c>
-      <c r="B386" t="s">
-        <v>209</v>
-      </c>
-      <c r="C386">
-        <v>868</v>
-      </c>
-      <c r="H386" t="s">
-        <v>64</v>
-      </c>
-      <c r="K386" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A387" t="s">
-        <v>278</v>
-      </c>
-      <c r="B387" t="s">
-        <v>209</v>
-      </c>
-      <c r="C387">
-        <v>872</v>
-      </c>
-      <c r="H387" t="s">
-        <v>85</v>
-      </c>
-      <c r="K387" s="1" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A388" t="s">
-        <v>278</v>
-      </c>
-      <c r="B388" t="s">
-        <v>209</v>
-      </c>
-      <c r="C388">
-        <v>872</v>
-      </c>
-      <c r="H388" t="s">
-        <v>85</v>
-      </c>
-      <c r="K388" s="1" t="s">
-        <v>211</v>
+      <c r="L373">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>